<commit_message>
Atualização da lista de Ecolas Municipais e Estaduais com a Localização
</commit_message>
<xml_diff>
--- a/dados/escolas.xlsx
+++ b/dados/escolas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\Desktop\Repositorio\ProjetosPessoais\CanoasTransito\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB32446-B6E8-48AA-9D29-DD1037CE3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67106812-AA91-4F39-A83F-666DB9C05E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90935E0F-B9E2-4B44-AFE3-01FF1F0A538E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="248">
   <si>
     <t>EMEF GOV LEONEL DE MOURA BRIZOLA</t>
   </si>
@@ -293,70 +293,493 @@
     <t>BAIRRO</t>
   </si>
   <si>
-    <t>-29.8827806</t>
-  </si>
-  <si>
-    <t>-51.1512837</t>
-  </si>
-  <si>
-    <t>-29.890795</t>
-  </si>
-  <si>
-    <t>-51.128923</t>
-  </si>
-  <si>
-    <t>-29.9045692</t>
-  </si>
-  <si>
-    <t>-51.1663098</t>
-  </si>
-  <si>
-    <t>-29.9599135</t>
-  </si>
-  <si>
-    <t>-51.1879344</t>
-  </si>
-  <si>
-    <t>-29.9343714</t>
-  </si>
-  <si>
-    <t>-51.1977556</t>
-  </si>
-  <si>
-    <t>-29.9475408</t>
-  </si>
-  <si>
-    <t>-51.1850963</t>
-  </si>
-  <si>
-    <t>-29.9031012</t>
-  </si>
-  <si>
-    <t>-51.1650502</t>
-  </si>
-  <si>
-    <t>-29.9238371</t>
-  </si>
-  <si>
-    <t>-51.1432678</t>
-  </si>
-  <si>
-    <t>-29.8981821</t>
-  </si>
-  <si>
-    <t>-51.1849507</t>
-  </si>
-  <si>
-    <t>-29.958046</t>
-  </si>
-  <si>
-    <t>-51.1931636</t>
-  </si>
-  <si>
-    <t>IDEB Iniciais</t>
-  </si>
-  <si>
     <t>IDEB Finais</t>
+  </si>
+  <si>
+    <t>-29.882613131660400</t>
+  </si>
+  <si>
+    <t>-29.890525226719900</t>
+  </si>
+  <si>
+    <t>-29.904387867494100</t>
+  </si>
+  <si>
+    <t>-29.959825222954</t>
+  </si>
+  <si>
+    <t>-29.93418082554840</t>
+  </si>
+  <si>
+    <t>-29.947350251388600</t>
+  </si>
+  <si>
+    <t>-29.90294776631120</t>
+  </si>
+  <si>
+    <t>-29.92373949069140</t>
+  </si>
+  <si>
+    <t>-29.89806586240850</t>
+  </si>
+  <si>
+    <t>-29.95788335816810</t>
+  </si>
+  <si>
+    <t>-29.928302806551800</t>
+  </si>
+  <si>
+    <t>-51.15132661939450</t>
+  </si>
+  <si>
+    <t>-51.126315917541700</t>
+  </si>
+  <si>
+    <t>-51.163681259869100</t>
+  </si>
+  <si>
+    <t>-51.18488743526020</t>
+  </si>
+  <si>
+    <t>-51.19513778870380</t>
+  </si>
+  <si>
+    <t>-51.18240338685070</t>
+  </si>
+  <si>
+    <t>-51.16185303155790</t>
+  </si>
+  <si>
+    <t>-51.14047832732730</t>
+  </si>
+  <si>
+    <t>-51.18191446409910</t>
+  </si>
+  <si>
+    <t>-51.1896874818179</t>
+  </si>
+  <si>
+    <t>-51.16517078870400</t>
+  </si>
+  <si>
+    <t>-29.917955093725592</t>
+  </si>
+  <si>
+    <t>-51.16924740404869</t>
+  </si>
+  <si>
+    <t>-29.936704314594774</t>
+  </si>
+  <si>
+    <t>-51.16866588870378</t>
+  </si>
+  <si>
+    <t>-29.95662205153374</t>
+  </si>
+  <si>
+    <t>-51.18547331939138</t>
+  </si>
+  <si>
+    <t>-29.913962782740157</t>
+  </si>
+  <si>
+    <t>-51.21283794690171</t>
+  </si>
+  <si>
+    <t>-29.932518510987357</t>
+  </si>
+  <si>
+    <t>-51.178383517539906</t>
+  </si>
+  <si>
+    <t>-29.964921648864333</t>
+  </si>
+  <si>
+    <t>-51.1928875812927</t>
+  </si>
+  <si>
+    <t>-29.94952729414292</t>
+  </si>
+  <si>
+    <t>-51.15779829716247</t>
+  </si>
+  <si>
+    <t>-29.908517975184793</t>
+  </si>
+  <si>
+    <t>-51.1897195193934</t>
+  </si>
+  <si>
+    <t>-29.92796402807509</t>
+  </si>
+  <si>
+    <t>-51.192566391081435</t>
+  </si>
+  <si>
+    <t>-29.925770896025764</t>
+  </si>
+  <si>
+    <t>-51.14679013473689</t>
+  </si>
+  <si>
+    <t>-29.96142405916497</t>
+  </si>
+  <si>
+    <t>-51.1690873352602</t>
+  </si>
+  <si>
+    <t>-29.906627478452805</t>
+  </si>
+  <si>
+    <t>-51.13099086595113</t>
+  </si>
+  <si>
+    <t>-29.94088402957186</t>
+  </si>
+  <si>
+    <t>-51.164876160392424</t>
+  </si>
+  <si>
+    <t>IDEB</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>-29.96402524769106</t>
+  </si>
+  <si>
+    <t>-51.184635208276426</t>
+  </si>
+  <si>
+    <t>-29.915627286430816</t>
+  </si>
+  <si>
+    <t>-51.185194048754035</t>
+  </si>
+  <si>
+    <t>-29.953845338619086</t>
+  </si>
+  <si>
+    <t>-51.18597736594892</t>
+  </si>
+  <si>
+    <t>-29.954401156614527</t>
+  </si>
+  <si>
+    <t>-51.17231050827691</t>
+  </si>
+  <si>
+    <t>-29.93992712206049</t>
+  </si>
+  <si>
+    <t>-51.17305603896594</t>
+  </si>
+  <si>
+    <t>-29.961377578923617</t>
+  </si>
+  <si>
+    <t>-51.18093453155532</t>
+  </si>
+  <si>
+    <t>-29.90028886585995</t>
+  </si>
+  <si>
+    <t>-51.169094429705666</t>
+  </si>
+  <si>
+    <t>-29.887382757296752</t>
+  </si>
+  <si>
+    <t>-51.18149722970646</t>
+  </si>
+  <si>
+    <t>-29.944116331664993</t>
+  </si>
+  <si>
+    <t>-51.1808162971628</t>
+  </si>
+  <si>
+    <t>-29.954262464955608</t>
+  </si>
+  <si>
+    <t>-51.16177724742485</t>
+  </si>
+  <si>
+    <t>-29.942161041205424</t>
+  </si>
+  <si>
+    <t>-51.18360748552354</t>
+  </si>
+  <si>
+    <t>-29.912896077464698</t>
+  </si>
+  <si>
+    <t>-51.20875048499996</t>
+  </si>
+  <si>
+    <t>-29.933920398764943</t>
+  </si>
+  <si>
+    <t>-51.160599879441655</t>
+  </si>
+  <si>
+    <t>-29.945785434316555</t>
+  </si>
+  <si>
+    <t>-51.1584734678019</t>
+  </si>
+  <si>
+    <t>-29.905594071540424</t>
+  </si>
+  <si>
+    <t>-51.17498002600074</t>
+  </si>
+  <si>
+    <t>-29.913689081362257</t>
+  </si>
+  <si>
+    <t>-51.19530441991809</t>
+  </si>
+  <si>
+    <t>-29.932673615765545</t>
+  </si>
+  <si>
+    <t>-51.15803590642541</t>
+  </si>
+  <si>
+    <t>-29.90931747623591</t>
+  </si>
+  <si>
+    <t>-51.20646209901692</t>
+  </si>
+  <si>
+    <t>-29.942504541879497</t>
+  </si>
+  <si>
+    <t>-51.191716477588955</t>
+  </si>
+  <si>
+    <t>-29.964333648094698</t>
+  </si>
+  <si>
+    <t>-51.20052453763741</t>
+  </si>
+  <si>
+    <t>-29.914755985047996</t>
+  </si>
+  <si>
+    <t>-51.1193309045739</t>
+  </si>
+  <si>
+    <t>-29.93164353804268</t>
+  </si>
+  <si>
+    <t>-51.17354110457306</t>
+  </si>
+  <si>
+    <t>-29.885701847415245</t>
+  </si>
+  <si>
+    <t>-51.17275778737853</t>
+  </si>
+  <si>
+    <t>-29.902099769650878</t>
+  </si>
+  <si>
+    <t>-51.20329661991863</t>
+  </si>
+  <si>
+    <t>-29.901660366768482</t>
+  </si>
+  <si>
+    <t>-51.21664601250903</t>
+  </si>
+  <si>
+    <t>-29.90119037294703</t>
+  </si>
+  <si>
+    <t>-51.17343208923025</t>
+  </si>
+  <si>
+    <t>-29.909545577473104</t>
+  </si>
+  <si>
+    <t>-51.191459658541426</t>
+  </si>
+  <si>
+    <t>-29.928624195708462</t>
+  </si>
+  <si>
+    <t>-51.15155782680221</t>
+  </si>
+  <si>
+    <t>-29.903918863771864</t>
+  </si>
+  <si>
+    <t>-51.21080793526272</t>
+  </si>
+  <si>
+    <t>-29.94667486441092</t>
+  </si>
+  <si>
+    <t>-51.17293643340847</t>
+  </si>
+  <si>
+    <t>-29.91921400745935</t>
+  </si>
+  <si>
+    <t>-51.17569421013092</t>
+  </si>
+  <si>
+    <t>-29.90077196356595</t>
+  </si>
+  <si>
+    <t>-51.22691689716489</t>
+  </si>
+  <si>
+    <t>-29.902110165564036</t>
+  </si>
+  <si>
+    <t>-51.189578505099284</t>
+  </si>
+  <si>
+    <t>-29.916931092524344</t>
+  </si>
+  <si>
+    <t>-51.20656466224594</t>
+  </si>
+  <si>
+    <t>-29.905696870672813</t>
+  </si>
+  <si>
+    <t>-51.22077330272186</t>
+  </si>
+  <si>
+    <t>-29.91894409964832</t>
+  </si>
+  <si>
+    <t>-51.1484082664756</t>
+  </si>
+  <si>
+    <t>-29.8824238265095</t>
+  </si>
+  <si>
+    <t>-51.17499061436217</t>
+  </si>
+  <si>
+    <t>-29.902220768023053</t>
+  </si>
+  <si>
+    <t>-51.13534426304917</t>
+  </si>
+  <si>
+    <t>-29.921776493682383</t>
+  </si>
+  <si>
+    <t>-51.18188021806537</t>
+  </si>
+  <si>
+    <t>-29.891466954405626</t>
+  </si>
+  <si>
+    <t>-51.1383350955904</t>
+  </si>
+  <si>
+    <t>-29.897847149443024</t>
+  </si>
+  <si>
+    <t>-51.138593435263054</t>
+  </si>
+  <si>
+    <t>-29.907479472889555</t>
+  </si>
+  <si>
+    <t>-51.14652006409874</t>
+  </si>
+  <si>
+    <t>-29.903269566821816</t>
+  </si>
+  <si>
+    <t>-51.199001225475854</t>
+  </si>
+  <si>
+    <t>-29.923700912195827</t>
+  </si>
+  <si>
+    <t>-51.130266596639</t>
+  </si>
+  <si>
+    <t>-29.914811655620916</t>
+  </si>
+  <si>
+    <t>-51.21534050671375</t>
+  </si>
+  <si>
+    <t>-29.92018248593792</t>
+  </si>
+  <si>
+    <t>-51.1446423566885</t>
+  </si>
+  <si>
+    <t>-29.896042658803996</t>
+  </si>
+  <si>
+    <t>-51.13456466224685</t>
+  </si>
+  <si>
+    <t>-29.921118693953638</t>
+  </si>
+  <si>
+    <t>-51.1211138008687</t>
+  </si>
+  <si>
+    <t>-29.8995267283447</t>
+  </si>
+  <si>
+    <t>-51.22450686040946</t>
+  </si>
+  <si>
+    <t>-29.911727877736208</t>
+  </si>
+  <si>
+    <t>-51.14276433526241</t>
+  </si>
+  <si>
+    <t>-29.901391363842137</t>
+  </si>
+  <si>
+    <t>-51.13884605298455</t>
+  </si>
+  <si>
+    <t>-29.888013335043045</t>
+  </si>
+  <si>
+    <t>-51.133471060394776</t>
+  </si>
+  <si>
+    <t>-29.902898865726545</t>
+  </si>
+  <si>
+    <t>-51.23270572785315</t>
+  </si>
+  <si>
+    <t>-29.91006337664886</t>
+  </si>
+  <si>
+    <t>-51.226846894787066</t>
   </si>
 </sst>
 </file>
@@ -745,7 +1168,7 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,8 +1176,9 @@
     <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="5" width="11.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -774,11 +1198,11 @@
       <c r="E1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>105</v>
+      <c r="F1" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -789,10 +1213,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
+      </c>
+      <c r="F2" s="2">
+        <v>7</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -808,7 +1235,10 @@
         <v>87</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -821,10 +1251,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -837,10 +1270,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -853,10 +1286,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -869,10 +1302,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -883,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -897,10 +1330,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -911,10 +1344,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -925,10 +1358,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -938,6 +1371,12 @@
       <c r="B12" t="s">
         <v>1</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -946,6 +1385,12 @@
       <c r="B13" t="s">
         <v>1</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -954,6 +1399,12 @@
       <c r="B14" t="s">
         <v>1</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -962,6 +1413,12 @@
       <c r="B15" t="s">
         <v>1</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -970,509 +1427,905 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D30" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D40" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D41" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D42" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D43" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D45" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D47" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D49" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D50" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D51" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D52" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D53" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D54" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D55" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D56" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D57" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D58" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D59" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D60" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D61" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D62" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D63" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D64" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D65" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D66" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D67" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D68" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D69" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D70" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D71" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D72" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D73" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D74" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D75" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D76" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D77" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D78" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>